<commit_message>
Added different buildings, npcs therein, and a storyline of sorts.
</commit_message>
<xml_diff>
--- a/Worlds/TTotalMap.xlsx
+++ b/Worlds/TTotalMap.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29532" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29532" uniqueCount="29">
   <si>
     <t>grass</t>
   </si>
@@ -88,6 +88,21 @@
   <si>
     <t>|</t>
   </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
 </sst>
 </file>
 
@@ -131,27 +146,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="88">
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color theme="6" tint="0.39994506668294322"/>
@@ -229,786 +224,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1409,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HI136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BU67" workbookViewId="0">
-      <selection activeCell="DK83" sqref="DK83"/>
+    <sheetView tabSelected="1" topLeftCell="CK103" workbookViewId="0">
+      <selection activeCell="DO117" sqref="DO117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53954,7 +53169,7 @@
         <v>2</v>
       </c>
       <c r="CU81" s="3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="CV81" s="3" t="s">
         <v>12</v>
@@ -55326,7 +54541,7 @@
         <v>2</v>
       </c>
       <c r="DQ83" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="DR83" s="3" t="s">
         <v>12</v>
@@ -60484,7 +59699,7 @@
         <v>2</v>
       </c>
       <c r="CU91" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="CV91" s="3" t="s">
         <v>12</v>
@@ -61104,7 +60319,7 @@
         <v>2</v>
       </c>
       <c r="CJ92" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="CK92" s="3" t="s">
         <v>12</v>
@@ -72478,7 +71693,7 @@
         <v>2</v>
       </c>
       <c r="FW109" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="FX109" s="3" t="s">
         <v>12</v>
@@ -72861,7 +72076,7 @@
         <v>2</v>
       </c>
       <c r="CK110" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="CL110" s="3" t="s">
         <v>12</v>
@@ -73814,7 +73029,7 @@
         <v>2</v>
       </c>
       <c r="GG111" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="GH111" s="3" t="s">
         <v>12</v>
@@ -76162,7 +75377,7 @@
         <v>2</v>
       </c>
       <c r="CW115" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="CX115" s="3" t="s">
         <v>12</v>
@@ -76225,7 +75440,7 @@
         <v>2</v>
       </c>
       <c r="DR115" s="3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="DS115" s="3" t="s">
         <v>12</v>
@@ -77687,7 +76902,7 @@
         <v>2</v>
       </c>
       <c r="FR117" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="FS117" s="3" t="s">
         <v>12</v>
@@ -78376,7 +77591,7 @@
         <v>2</v>
       </c>
       <c r="GD118" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="GE118" s="3" t="s">
         <v>12</v>
@@ -78963,7 +78178,7 @@
         <v>2</v>
       </c>
       <c r="FH119" s="3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="FI119" s="3" t="s">
         <v>12</v>
@@ -80365,7 +79580,7 @@
         <v>2</v>
       </c>
       <c r="GN121" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="GO121" s="3" t="s">
         <v>12</v>
@@ -90228,34 +89443,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="CH21">
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"g"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS1:EQ67 BS68:BX68 EA68:ED68 EJ68:EQ68 CG68:CI68 CN68:CO68 CT68:CU68 CZ68:DR68">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"t"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"g"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"t"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"g"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:HI136">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"r"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"b"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"f"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>